<commit_message>
adding controls reference and Requirement interface
</commit_message>
<xml_diff>
--- a/requirements.xlsx
+++ b/requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sean/Source/my-cli-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE197565-D322-A84E-8397-76ED631D7B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C432F962-9DE4-CD4F-BDBE-F2DB87CC9BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16620" xr2:uid="{253DE04B-6921-F94F-A23C-A907349A208E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>ID</t>
   </si>
@@ -60,9 +60,6 @@
   </si>
   <si>
     <t>The application should use the NIST instance of Okta for athentication.</t>
-  </si>
-  <si>
-    <t>Controls Reference</t>
   </si>
   <si>
     <t>Logout</t>
@@ -70,6 +67,15 @@
   <si>
     <t>The application should allow logout of the application
 as well as selecting to logout og the Okta login server.</t>
+  </si>
+  <si>
+    <t>AC-11, AC-12</t>
+  </si>
+  <si>
+    <t>IA-2</t>
+  </si>
+  <si>
+    <t>Controls_Reference</t>
   </si>
 </sst>
 </file>
@@ -427,7 +433,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -451,7 +457,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -467,6 +473,9 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -481,6 +490,9 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -490,10 +502,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>